<commit_message>
Update batch file creator and GAMS file
</commit_message>
<xml_diff>
--- a/data_files/Resolution_values.xlsx
+++ b/data_files/Resolution_values.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -52,7 +52,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +357,7 @@
   <dimension ref="B3:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>